<commit_message>
Simplify logging system configuration
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I495"/>
+  <dimension ref="A1:I504"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18760,6 +18760,339 @@
         <v>400</v>
       </c>
       <c r="I495" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="n">
+        <v>45721.72894113426</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E496" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F496" t="n">
+        <v>400</v>
+      </c>
+      <c r="G496" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H496" t="n">
+        <v>400</v>
+      </c>
+      <c r="I496" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="2" t="n">
+        <v>45721.72896428241</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F497" t="n">
+        <v>400</v>
+      </c>
+      <c r="G497" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H497" t="n">
+        <v>400</v>
+      </c>
+      <c r="I497" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="2" t="n">
+        <v>45721.72898766203</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F498" t="n">
+        <v>400</v>
+      </c>
+      <c r="G498" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H498" t="n">
+        <v>400</v>
+      </c>
+      <c r="I498" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="2" t="n">
+        <v>45722.22908445602</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E499" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F499" t="n">
+        <v>400</v>
+      </c>
+      <c r="G499" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H499" t="n">
+        <v>400</v>
+      </c>
+      <c r="I499" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="2" t="n">
+        <v>45722.22910648148</v>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E500" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F500" t="n">
+        <v>400</v>
+      </c>
+      <c r="G500" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H500" t="n">
+        <v>400</v>
+      </c>
+      <c r="I500" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="2" t="n">
+        <v>45722.22912973379</v>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E501" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F501" t="n">
+        <v>400</v>
+      </c>
+      <c r="G501" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H501" t="n">
+        <v>400</v>
+      </c>
+      <c r="I501" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="2" t="n">
+        <v>45723.19113143518</v>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F502" t="n">
+        <v>400</v>
+      </c>
+      <c r="G502" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H502" t="n">
+        <v>400</v>
+      </c>
+      <c r="I502" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="2" t="n">
+        <v>45723.19115481481</v>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F503" t="n">
+        <v>400</v>
+      </c>
+      <c r="G503" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H503" t="n">
+        <v>400</v>
+      </c>
+      <c r="I503" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="2" t="n">
+        <v>45723.19117797454</v>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F504" t="n">
+        <v>400</v>
+      </c>
+      <c r="G504" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H504" t="n">
+        <v>400</v>
+      </c>
+      <c r="I504" t="n">
         <v>13</v>
       </c>
     </row>
@@ -18774,7 +19107,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I373"/>
+  <dimension ref="A1:I382"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32590,6 +32923,339 @@
         <v>400</v>
       </c>
       <c r="I373" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="2" t="n">
+        <v>45721.72988806713</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F374" t="n">
+        <v>400</v>
+      </c>
+      <c r="G374" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H374" t="n">
+        <v>400</v>
+      </c>
+      <c r="I374" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="2" t="n">
+        <v>45721.72991133102</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F375" t="n">
+        <v>400</v>
+      </c>
+      <c r="G375" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H375" t="n">
+        <v>400</v>
+      </c>
+      <c r="I375" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="2" t="n">
+        <v>45721.72993467592</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F376" t="n">
+        <v>400</v>
+      </c>
+      <c r="G376" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H376" t="n">
+        <v>400</v>
+      </c>
+      <c r="I376" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="2" t="n">
+        <v>45722.23020512731</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F377" t="n">
+        <v>400</v>
+      </c>
+      <c r="G377" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H377" t="n">
+        <v>400</v>
+      </c>
+      <c r="I377" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="2" t="n">
+        <v>45722.23022724537</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F378" t="n">
+        <v>400</v>
+      </c>
+      <c r="G378" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H378" t="n">
+        <v>400</v>
+      </c>
+      <c r="I378" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="2" t="n">
+        <v>45722.23025050926</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F379" t="n">
+        <v>400</v>
+      </c>
+      <c r="G379" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H379" t="n">
+        <v>400</v>
+      </c>
+      <c r="I379" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="2" t="n">
+        <v>45723.19124234954</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F380" t="n">
+        <v>400</v>
+      </c>
+      <c r="G380" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H380" t="n">
+        <v>400</v>
+      </c>
+      <c r="I380" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="2" t="n">
+        <v>45723.19126548611</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F381" t="n">
+        <v>400</v>
+      </c>
+      <c r="G381" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H381" t="n">
+        <v>400</v>
+      </c>
+      <c r="I381" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="2" t="n">
+        <v>45723.19128880787</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F382" t="n">
+        <v>400</v>
+      </c>
+      <c r="G382" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H382" t="n">
+        <v>400</v>
+      </c>
+      <c r="I382" t="n">
         <v>14</v>
       </c>
     </row>
@@ -32604,7 +33270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I406"/>
+  <dimension ref="A1:I415"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47641,6 +48307,339 @@
         <v>400</v>
       </c>
       <c r="I406" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="2" t="n">
+        <v>45721.72979079861</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F407" t="n">
+        <v>400</v>
+      </c>
+      <c r="G407" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H407" t="n">
+        <v>400</v>
+      </c>
+      <c r="I407" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="2" t="n">
+        <v>45721.72981402778</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F408" t="n">
+        <v>400</v>
+      </c>
+      <c r="G408" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H408" t="n">
+        <v>400</v>
+      </c>
+      <c r="I408" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="2" t="n">
+        <v>45721.7298375463</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F409" t="n">
+        <v>400</v>
+      </c>
+      <c r="G409" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H409" t="n">
+        <v>400</v>
+      </c>
+      <c r="I409" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="2" t="n">
+        <v>45722.23010768519</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F410" t="n">
+        <v>400</v>
+      </c>
+      <c r="G410" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H410" t="n">
+        <v>400</v>
+      </c>
+      <c r="I410" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="2" t="n">
+        <v>45722.23012966435</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F411" t="n">
+        <v>400</v>
+      </c>
+      <c r="G411" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H411" t="n">
+        <v>400</v>
+      </c>
+      <c r="I411" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="2" t="n">
+        <v>45722.23015302084</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F412" t="n">
+        <v>400</v>
+      </c>
+      <c r="G412" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H412" t="n">
+        <v>400</v>
+      </c>
+      <c r="I412" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="2" t="n">
+        <v>45723.19132489583</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F413" t="n">
+        <v>400</v>
+      </c>
+      <c r="G413" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H413" t="n">
+        <v>400</v>
+      </c>
+      <c r="I413" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="2" t="n">
+        <v>45723.19134847222</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F414" t="n">
+        <v>400</v>
+      </c>
+      <c r="G414" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H414" t="n">
+        <v>400</v>
+      </c>
+      <c r="I414" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="2" t="n">
+        <v>45723.19137149306</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x06,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>0xff</t>
+        </is>
+      </c>
+      <c r="F415" t="n">
+        <v>400</v>
+      </c>
+      <c r="G415" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H415" t="n">
+        <v>400</v>
+      </c>
+      <c r="I415" t="n">
         <v>255</v>
       </c>
     </row>
@@ -47655,7 +48654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I376"/>
+  <dimension ref="A1:I388"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -61585,6 +62584,450 @@
         <v>3</v>
       </c>
     </row>
+    <row r="377">
+      <c r="A377" s="2" t="n">
+        <v>45721.72820228009</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F377" t="n">
+        <v>400</v>
+      </c>
+      <c r="G377" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H377" t="n">
+        <v>400</v>
+      </c>
+      <c r="I377" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="2" t="n">
+        <v>45721.7282258449</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F378" t="n">
+        <v>400</v>
+      </c>
+      <c r="G378" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H378" t="n">
+        <v>400</v>
+      </c>
+      <c r="I378" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="2" t="n">
+        <v>45721.72824888889</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F379" t="n">
+        <v>400</v>
+      </c>
+      <c r="G379" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H379" t="n">
+        <v>400</v>
+      </c>
+      <c r="I379" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="2" t="n">
+        <v>45722.22834673611</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F380" t="n">
+        <v>400</v>
+      </c>
+      <c r="G380" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H380" t="n">
+        <v>400</v>
+      </c>
+      <c r="I380" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="2" t="n">
+        <v>45722.22836789352</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F381" t="n">
+        <v>400</v>
+      </c>
+      <c r="G381" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H381" t="n">
+        <v>400</v>
+      </c>
+      <c r="I381" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="2" t="n">
+        <v>45722.22839168982</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F382" t="n">
+        <v>400</v>
+      </c>
+      <c r="G382" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H382" t="n">
+        <v>400</v>
+      </c>
+      <c r="I382" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="2" t="n">
+        <v>45722.72848770834</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F383" t="n">
+        <v>400</v>
+      </c>
+      <c r="G383" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H383" t="n">
+        <v>400</v>
+      </c>
+      <c r="I383" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="2" t="n">
+        <v>45722.72850997685</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F384" t="n">
+        <v>400</v>
+      </c>
+      <c r="G384" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H384" t="n">
+        <v>400</v>
+      </c>
+      <c r="I384" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="2" t="n">
+        <v>45722.72853335648</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F385" t="n">
+        <v>400</v>
+      </c>
+      <c r="G385" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H385" t="n">
+        <v>400</v>
+      </c>
+      <c r="I385" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="2" t="n">
+        <v>45723.22863142361</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F386" t="n">
+        <v>400</v>
+      </c>
+      <c r="G386" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H386" t="n">
+        <v>400</v>
+      </c>
+      <c r="I386" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2" t="n">
+        <v>45723.22865329861</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F387" t="n">
+        <v>400</v>
+      </c>
+      <c r="G387" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H387" t="n">
+        <v>400</v>
+      </c>
+      <c r="I387" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="2" t="n">
+        <v>45723.22867643519</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F388" t="n">
+        <v>400</v>
+      </c>
+      <c r="G388" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H388" t="n">
+        <v>400</v>
+      </c>
+      <c r="I388" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise build script optimization
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1375,966 +1375,123 @@
         <v>13</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45729.23225322917</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>400</v>
+      </c>
+      <c r="I26" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45729.23227436343</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>400</v>
+      </c>
+      <c r="I27" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45729.23229758102</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x14,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0xd</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>400</v>
+      </c>
+      <c r="I28" t="n">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>总长</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>实际长度</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>和校验</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>总长_DEC</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ID_DEC</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>实际长度_DEC</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>和校验_DEC</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45725.07909302083</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>400</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H2" t="n">
-        <v>400</v>
-      </c>
-      <c r="I2" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45725.07911518519</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>400</v>
-      </c>
-      <c r="G3" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H3" t="n">
-        <v>400</v>
-      </c>
-      <c r="I3" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45725.07913833333</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>400</v>
-      </c>
-      <c r="G4" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H4" t="n">
-        <v>400</v>
-      </c>
-      <c r="I4" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45725.57923533564</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>400</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H5" t="n">
-        <v>400</v>
-      </c>
-      <c r="I5" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45725.57925716435</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>400</v>
-      </c>
-      <c r="G6" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H6" t="n">
-        <v>400</v>
-      </c>
-      <c r="I6" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45725.57928042824</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>400</v>
-      </c>
-      <c r="G7" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H7" t="n">
-        <v>400</v>
-      </c>
-      <c r="I7" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45726.07937777778</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>400</v>
-      </c>
-      <c r="G8" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H8" t="n">
-        <v>400</v>
-      </c>
-      <c r="I8" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45726.07939922454</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>400</v>
-      </c>
-      <c r="G9" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H9" t="n">
-        <v>400</v>
-      </c>
-      <c r="I9" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45726.07942256945</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>400</v>
-      </c>
-      <c r="G10" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H10" t="n">
-        <v>400</v>
-      </c>
-      <c r="I10" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45726.57952</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>400</v>
-      </c>
-      <c r="G11" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H11" t="n">
-        <v>400</v>
-      </c>
-      <c r="I11" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>45726.57954204861</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>400</v>
-      </c>
-      <c r="G12" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H12" t="n">
-        <v>400</v>
-      </c>
-      <c r="I12" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>45726.57956549768</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>400</v>
-      </c>
-      <c r="G13" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H13" t="n">
-        <v>400</v>
-      </c>
-      <c r="I13" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>45727.07966211806</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>400</v>
-      </c>
-      <c r="G14" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H14" t="n">
-        <v>400</v>
-      </c>
-      <c r="I14" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>45727.07968420139</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>400</v>
-      </c>
-      <c r="G15" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H15" t="n">
-        <v>400</v>
-      </c>
-      <c r="I15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>45727.07970724537</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>400</v>
-      </c>
-      <c r="G16" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H16" t="n">
-        <v>400</v>
-      </c>
-      <c r="I16" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>45727.57980457176</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>400</v>
-      </c>
-      <c r="G17" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H17" t="n">
-        <v>400</v>
-      </c>
-      <c r="I17" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>45727.57982650463</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>400</v>
-      </c>
-      <c r="G18" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H18" t="n">
-        <v>400</v>
-      </c>
-      <c r="I18" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>45727.57985059028</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0x01,0x90,</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>0xe</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>400</v>
-      </c>
-      <c r="G19" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H19" t="n">
-        <v>400</v>
-      </c>
-      <c r="I19" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>45728.07994677083</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>400</v>
-      </c>
-      <c r="G20" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H20" t="n">
-        <v>390</v>
-      </c>
-      <c r="I20" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>45728.07996869213</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>400</v>
-      </c>
-      <c r="G21" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H21" t="n">
-        <v>390</v>
-      </c>
-      <c r="I21" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>45728.07999162037</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>400</v>
-      </c>
-      <c r="G22" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H22" t="n">
-        <v>390</v>
-      </c>
-      <c r="I22" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>45728.58008952547</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>400</v>
-      </c>
-      <c r="G23" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H23" t="n">
-        <v>390</v>
-      </c>
-      <c r="I23" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
-        <v>45728.5801115625</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>400</v>
-      </c>
-      <c r="G24" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H24" t="n">
-        <v>390</v>
-      </c>
-      <c r="I24" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>45728.58013472222</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>0x01,0x90</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0x01,0x86,</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0x4</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>400</v>
-      </c>
-      <c r="G25" t="n">
-        <v>5.686312626471138e+23</v>
-      </c>
-      <c r="H25" t="n">
-        <v>390</v>
-      </c>
-      <c r="I25" t="n">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2397,6 +1554,1071 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
+        <v>45725.07909302083</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>400</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H2" t="n">
+        <v>400</v>
+      </c>
+      <c r="I2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45725.07911518519</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>400</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H3" t="n">
+        <v>400</v>
+      </c>
+      <c r="I3" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45725.07913833333</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>400</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H4" t="n">
+        <v>400</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45725.57923533564</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>400</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H5" t="n">
+        <v>400</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45725.57925716435</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>400</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I6" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45725.57928042824</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>400</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H7" t="n">
+        <v>400</v>
+      </c>
+      <c r="I7" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45726.07937777778</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>400</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H8" t="n">
+        <v>400</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45726.07939922454</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>400</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H9" t="n">
+        <v>400</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45726.07942256945</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>400</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H10" t="n">
+        <v>400</v>
+      </c>
+      <c r="I10" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45726.57952</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>400</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H11" t="n">
+        <v>400</v>
+      </c>
+      <c r="I11" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45726.57954204861</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>400</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H12" t="n">
+        <v>400</v>
+      </c>
+      <c r="I12" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45726.57956549768</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>400</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H13" t="n">
+        <v>400</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45727.07966211806</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>400</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H14" t="n">
+        <v>400</v>
+      </c>
+      <c r="I14" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45727.07968420139</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>400</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H15" t="n">
+        <v>400</v>
+      </c>
+      <c r="I15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45727.07970724537</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>400</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H16" t="n">
+        <v>400</v>
+      </c>
+      <c r="I16" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45727.57980457176</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>400</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H17" t="n">
+        <v>400</v>
+      </c>
+      <c r="I17" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45727.57982650463</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>400</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H18" t="n">
+        <v>400</v>
+      </c>
+      <c r="I18" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45727.57985059028</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>400</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H19" t="n">
+        <v>400</v>
+      </c>
+      <c r="I19" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45728.07994677083</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>400</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H20" t="n">
+        <v>390</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45728.07996869213</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>400</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H21" t="n">
+        <v>390</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45728.07999162037</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>400</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H22" t="n">
+        <v>390</v>
+      </c>
+      <c r="I22" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45728.58008952547</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>400</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H23" t="n">
+        <v>390</v>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45728.5801115625</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>400</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>390</v>
+      </c>
+      <c r="I24" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45728.58013472222</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>400</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H25" t="n">
+        <v>390</v>
+      </c>
+      <c r="I25" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45729.08023151621</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>390</v>
+      </c>
+      <c r="I26" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45729.08025335648</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>400</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>390</v>
+      </c>
+      <c r="I27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>45729.08027658565</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x15,0x41,0x0c,</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0x01,0x86,</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0x4</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>400</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H28" t="n">
+        <v>390</v>
+      </c>
+      <c r="I28" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>总长</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>实际长度</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>和校验</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>总长_DEC</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ID_DEC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>实际长度_DEC</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>和校验_DEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>45725.22919952546</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -3391,6 +3613,117 @@
         <v>400</v>
       </c>
       <c r="I28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45729.26805734954</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>400</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H29" t="n">
+        <v>400</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45729.26807929398</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>400</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H30" t="n">
+        <v>400</v>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45729.26810284722</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>400</v>
+      </c>
+      <c r="I31" t="n">
         <v>3</v>
       </c>
     </row>
@@ -3405,7 +3738,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4459,6 +4792,117 @@
         <v>3</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45729.26805734954</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>400</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H29" t="n">
+        <v>400</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>45729.26807929398</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>400</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H30" t="n">
+        <v>400</v>
+      </c>
+      <c r="I30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45729.26810284722</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x90</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x90,</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>400</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.686312626471138e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>400</v>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>